<commit_message>
updated the jars and code, data provider still pending
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/SignIn.xlsx
+++ b/src/test/resources/TestData/SignIn.xlsx
@@ -3,12 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FB8A49E-F161-4134-BB05-38D38B21755D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11E556F2-3395-4CFE-A9CC-F952DCF9F550}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="SignIn Data" sheetId="1" r:id="rId1"/>
+    <sheet name="SignIn_Data_Positive" sheetId="1" r:id="rId1"/>
+    <sheet name="SignIn_Data_Negative" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
   <si>
     <t>EmailID</t>
   </si>
@@ -31,7 +32,13 @@
     <t>tripti.shende@ymail.com</t>
   </si>
   <si>
-    <t>Tripu@1993</t>
+    <t>Tripu1993</t>
+  </si>
+  <si>
+    <t>triptishende@gmail.com</t>
+  </si>
+  <si>
+    <t>Tripti1993</t>
   </si>
 </sst>
 </file>
@@ -363,13 +370,13 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -384,14 +391,59 @@
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" t="s">
         <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{13C28136-E982-4969-8B9F-E89A9C05B052}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{56D0824C-6A1A-43AA-B3D0-AB9339B5CDA9}"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{AF3D11BC-406F-48A9-8A51-E1AE62E87B58}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BC7FC1-7861-4936-B11C-567B574D520A}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{9316A627-5221-48A0-87E2-8AB826FAECCC}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{1AD4213D-77A2-4B0B-BAB9-1482277735B8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
AddToCart test and page with generic xpaths
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData/SignIn.xlsx
+++ b/src/test/resources/TestData/SignIn.xlsx
@@ -3,14 +3,15 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36341EA4-73DE-4756-88A1-79C759E8AED3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8BD7AB9-C6F9-4CB6-BB15-BEEF0EF223CE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SignIn_Data_Positive" sheetId="1" r:id="rId1"/>
     <sheet name="Product Details" sheetId="3" r:id="rId2"/>
-    <sheet name="SignIn_Data_Negative" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId3"/>
+    <sheet name="SignIn_Data_Negative" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>EmailID</t>
   </si>
@@ -60,9 +61,6 @@
     <t>Quantity</t>
   </si>
   <si>
-    <t>Sports</t>
-  </si>
-  <si>
     <t>BRUNTON ECLIPSE COMPASS</t>
   </si>
   <si>
@@ -75,10 +73,16 @@
     <t>HP TOUCHSMART</t>
   </si>
   <si>
-    <t>Apparels</t>
-  </si>
-  <si>
     <t>PURE COTTON T-SHIRT</t>
+  </si>
+  <si>
+    <t>Sport</t>
+  </si>
+  <si>
+    <t>Apparel</t>
+  </si>
+  <si>
+    <t>133</t>
   </si>
 </sst>
 </file>
@@ -123,10 +127,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -446,13 +451,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FEB97BB4-00E2-4C99-B9FE-ECBA6C82AA35}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
@@ -476,58 +489,20 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="2">
-        <v>133</v>
+        <v>12</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="E2" s="2">
         <v>49.95</v>
       </c>
       <c r="F2" s="2">
         <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="2">
-        <v>31</v>
-      </c>
-      <c r="E3" s="2">
-        <v>799.99</v>
-      </c>
-      <c r="F3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="2">
-        <v>47</v>
-      </c>
-      <c r="E4" s="2">
-        <v>13.99</v>
-      </c>
-      <c r="F4" s="2">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -537,6 +512,59 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0D5CDB4-A14D-4099-B681-0007814237CF}">
+  <dimension ref="C5:H6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:H6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="2">
+        <v>31</v>
+      </c>
+      <c r="G5" s="2">
+        <v>799.99</v>
+      </c>
+      <c r="H5" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="2">
+        <v>47</v>
+      </c>
+      <c r="G6" s="2">
+        <v>13.99</v>
+      </c>
+      <c r="H6" s="2">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96BC7FC1-7861-4936-B11C-567B574D520A}">
   <dimension ref="A1:B3"/>
   <sheetViews>

</xml_diff>